<commit_message>
add some new phrases
</commit_message>
<xml_diff>
--- a/vectorize_data.xlsx
+++ b/vectorize_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yahry\PycharmProjects\DonSTU_Helper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minil\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="12000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="174">
   <si>
     <t>Context</t>
   </si>
@@ -438,6 +438,114 @@
   </si>
   <si>
     <t>что выходит</t>
+  </si>
+  <si>
+    <t>зачётка</t>
+  </si>
+  <si>
+    <t>покажи мою зачётку</t>
+  </si>
+  <si>
+    <t>покажи зачётку</t>
+  </si>
+  <si>
+    <t>пришли зачётку</t>
+  </si>
+  <si>
+    <t>пришли мне зачётку</t>
+  </si>
+  <si>
+    <t>пришли мою зачётку</t>
+  </si>
+  <si>
+    <t>пришли мне мою зачётку</t>
+  </si>
+  <si>
+    <t>итоги</t>
+  </si>
+  <si>
+    <t>мои итоги</t>
+  </si>
+  <si>
+    <t>что в полугодии</t>
+  </si>
+  <si>
+    <t>что выходит в полугодии</t>
+  </si>
+  <si>
+    <t>ведомость</t>
+  </si>
+  <si>
+    <t>дневник</t>
+  </si>
+  <si>
+    <t>покажи ведомость</t>
+  </si>
+  <si>
+    <t>покажи дневник</t>
+  </si>
+  <si>
+    <t>покажи результаты</t>
+  </si>
+  <si>
+    <t>пришли результаты</t>
+  </si>
+  <si>
+    <t>пришли результаты за полугодие</t>
+  </si>
+  <si>
+    <t>результаты за полугодие</t>
+  </si>
+  <si>
+    <t>открой оценки</t>
+  </si>
+  <si>
+    <t>открой ведомость</t>
+  </si>
+  <si>
+    <t>открой успеваемость</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> открой зачётку</t>
+  </si>
+  <si>
+    <t>открой результаты</t>
+  </si>
+  <si>
+    <t>что по стипендии</t>
+  </si>
+  <si>
+    <t>результаты</t>
+  </si>
+  <si>
+    <t>что выходит за семестр</t>
+  </si>
+  <si>
+    <t>семестр</t>
+  </si>
+  <si>
+    <t>оценки дай</t>
+  </si>
+  <si>
+    <t>выведи оценки</t>
+  </si>
+  <si>
+    <t>за что меня отчисляют</t>
+  </si>
+  <si>
+    <t>за что меня отчислят</t>
+  </si>
+  <si>
+    <t>мои долги</t>
+  </si>
+  <si>
+    <t>лист оценок</t>
+  </si>
+  <si>
+    <t>список оценок</t>
+  </si>
+  <si>
+    <t>Что мне поставили?</t>
   </si>
 </sst>
 </file>
@@ -591,7 +699,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -607,9 +715,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -647,7 +755,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -719,7 +827,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -869,10 +977,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E164"/>
+  <dimension ref="A1:E200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E137" sqref="E137"/>
+    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B199" sqref="B199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1529,21 +1637,33 @@
       <c r="A79" t="s">
         <v>115</v>
       </c>
+      <c r="B79" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>116</v>
       </c>
+      <c r="B80" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>117</v>
       </c>
+      <c r="B81" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>118</v>
       </c>
+      <c r="B82" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
@@ -2118,6 +2238,294 @@
         <v>136</v>
       </c>
       <c r="B164" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>165</v>
+      </c>
+      <c r="B165" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>138</v>
+      </c>
+      <c r="B166" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>139</v>
+      </c>
+      <c r="B167" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>140</v>
+      </c>
+      <c r="B168" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>141</v>
+      </c>
+      <c r="B169" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>142</v>
+      </c>
+      <c r="B170" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>143</v>
+      </c>
+      <c r="B171" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>144</v>
+      </c>
+      <c r="B172" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>145</v>
+      </c>
+      <c r="B173" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>146</v>
+      </c>
+      <c r="B174" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>147</v>
+      </c>
+      <c r="B175" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>148</v>
+      </c>
+      <c r="B176" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>149</v>
+      </c>
+      <c r="B177" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>150</v>
+      </c>
+      <c r="B178" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>151</v>
+      </c>
+      <c r="B179" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>152</v>
+      </c>
+      <c r="B180" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>163</v>
+      </c>
+      <c r="B181" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>153</v>
+      </c>
+      <c r="B182" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>154</v>
+      </c>
+      <c r="B183" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>155</v>
+      </c>
+      <c r="B184" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>156</v>
+      </c>
+      <c r="B185" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>157</v>
+      </c>
+      <c r="B186" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>158</v>
+      </c>
+      <c r="B187" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>159</v>
+      </c>
+      <c r="B188" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>160</v>
+      </c>
+      <c r="B189" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>161</v>
+      </c>
+      <c r="B190" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>162</v>
+      </c>
+      <c r="B191" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>164</v>
+      </c>
+      <c r="B192" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>166</v>
+      </c>
+      <c r="B193" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>167</v>
+      </c>
+      <c r="B194" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>168</v>
+      </c>
+      <c r="B195" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>169</v>
+      </c>
+      <c r="B196" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>170</v>
+      </c>
+      <c r="B197" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>171</v>
+      </c>
+      <c r="B198" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>172</v>
+      </c>
+      <c r="B199" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>173</v>
+      </c>
+      <c r="B200" s="2">
         <v>2</v>
       </c>
     </row>

</xml_diff>